<commit_message>
Analysis of results updated
</commit_message>
<xml_diff>
--- a/Tables-and-figures-of-results.xlsx
+++ b/Tables-and-figures-of-results.xlsx
@@ -1,57 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\Applying-GENRE-on-MaCoCu-bilingual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tajak\Google Drive\GitHub\Applying-GENRE-on-MaCoCu-bilingual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990CDFDE-85BB-47FF-91A1-F19CAEE1A4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA437B7B-287A-4FED-96A1-E9DD1167AECF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BC1F8B3F-D1EE-42C3-9CDD-4A0C35F3AB58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{BC1F8B3F-D1EE-42C3-9CDD-4A0C35F3AB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison of datasets" sheetId="1" r:id="rId1"/>
-    <sheet name="Sizes of datasets" sheetId="5" r:id="rId2"/>
-    <sheet name="Length difference" sheetId="7" r:id="rId3"/>
-    <sheet name="English-dist" sheetId="8" r:id="rId4"/>
-    <sheet name="Distr in MK" sheetId="6" r:id="rId5"/>
-    <sheet name="Distr in IS" sheetId="2" r:id="rId6"/>
-    <sheet name="Distr in MT" sheetId="4" r:id="rId7"/>
-    <sheet name="Distr in SL" sheetId="3" r:id="rId8"/>
-    <sheet name="Distr in TR" sheetId="9" r:id="rId9"/>
-    <sheet name="Distr in BG" sheetId="10" r:id="rId10"/>
+    <sheet name="Comparison of distribution" sheetId="11" r:id="rId2"/>
+    <sheet name="Sizes of datasets" sheetId="5" r:id="rId3"/>
+    <sheet name="Length difference" sheetId="7" r:id="rId4"/>
+    <sheet name="English-dist" sheetId="8" r:id="rId5"/>
+    <sheet name="Distr in MK" sheetId="6" r:id="rId6"/>
+    <sheet name="Distr in IS" sheetId="2" r:id="rId7"/>
+    <sheet name="Distr in MT" sheetId="4" r:id="rId8"/>
+    <sheet name="Distr in SL" sheetId="3" r:id="rId9"/>
+    <sheet name="Distr in TR" sheetId="9" r:id="rId10"/>
+    <sheet name="Distr in BG" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Distr in BG'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Distr in IS'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Distr in MK'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Distr in MT'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Distr in SL'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Distr in TR'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Distr in BG'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Distr in IS'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Distr in MK'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Distr in MT'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Distr in SL'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Distr in TR'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="155">
   <si>
     <t>MaCoCu-sl-en</t>
   </si>
@@ -498,13 +490,31 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>News (46%)</t>
+  </si>
+  <si>
+    <t>Promotion (38%)</t>
+  </si>
+  <si>
+    <t>Promotion (39%)</t>
+  </si>
+  <si>
+    <t>Genre much more present than in others</t>
+  </si>
+  <si>
+    <t>Legal (28%), News (35%)</t>
+  </si>
+  <si>
+    <t>Promotion (32%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +605,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -629,7 +652,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -752,6 +775,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8367,7 +8408,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3A209A79-BC7C-4322-BAF1-6C8194B8FA3E}" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3A209A79-BC7C-4322-BAF1-6C8194B8FA3E}" name="Table2" displayName="Table2" ref="A1:G10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D58A66D7-2CB2-4DA0-9C7C-F112EDF3FD0C}" name="Dataset" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{817841C7-8300-4EE5-A7EB-4612110B8591}" name="MaCoCu-sl-en" dataDxfId="5"/>
@@ -8678,24 +8719,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1544E46A-78C9-4250-9787-2ED89FE698E6}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="18.36328125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="29.453125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="29.44140625" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8718,7 +8759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="15.6">
       <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
@@ -8741,7 +8782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="15.6">
       <c r="A3" s="39" t="s">
         <v>3</v>
       </c>
@@ -8764,7 +8805,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="15.6">
       <c r="A4" s="39" t="s">
         <v>7</v>
       </c>
@@ -8787,7 +8828,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="15.6">
       <c r="A5" s="39" t="s">
         <v>11</v>
       </c>
@@ -8810,7 +8851,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="15.6">
       <c r="A6" s="39" t="s">
         <v>4</v>
       </c>
@@ -8833,7 +8874,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="30.6">
       <c r="A7" s="39" t="s">
         <v>44</v>
       </c>
@@ -8856,7 +8897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="15.6">
       <c r="A8" s="39" t="s">
         <v>47</v>
       </c>
@@ -8879,7 +8920,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="39" t="s">
         <v>43</v>
       </c>
@@ -8902,89 +8943,110 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30.6">
+      <c r="A10" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="13"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8996,19 +9058,117 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0970C1-54A1-466F-8B11-808A46DDE000}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="27" style="34" customWidth="1"/>
+    <col min="2" max="3" width="21.21875" style="34" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="33">
+        <v>0.277673</v>
+      </c>
+      <c r="C2" s="33"/>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="33">
+        <v>0.16120699999999999</v>
+      </c>
+      <c r="C3" s="33"/>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="33">
+        <v>3.1772800000000004E-2</v>
+      </c>
+      <c r="C4" s="33"/>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="33">
+        <v>0.134713</v>
+      </c>
+      <c r="C5" s="33"/>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1.3107500000000001E-2</v>
+      </c>
+      <c r="C6" s="33"/>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="33">
+        <v>0.37993199999999999</v>
+      </c>
+      <c r="C7" s="33"/>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="33">
+        <v>1.59458E-3</v>
+      </c>
+      <c r="C8" s="33"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{FE0970C1-54A1-466F-8B11-808A46DDE000}">
+    <sortState ref="A2:D8">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1343A133-63B5-47F9-820E-915378298B5C}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="29.36328125" style="34" customWidth="1"/>
+    <col min="1" max="2" width="29.33203125" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="29" t="s">
         <v>62</v>
       </c>
@@ -9016,7 +9176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" s="32" t="s">
         <v>15</v>
       </c>
@@ -9024,7 +9184,7 @@
         <v>0.23852499999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15">
       <c r="A3" s="32" t="s">
         <v>17</v>
       </c>
@@ -9032,7 +9192,7 @@
         <v>7.6639899999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15">
       <c r="A4" s="32" t="s">
         <v>19</v>
       </c>
@@ -9040,7 +9200,7 @@
         <v>3.0696599999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15">
       <c r="A5" s="32" t="s">
         <v>16</v>
       </c>
@@ -9048,7 +9208,7 @@
         <v>0.191916</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
@@ -9056,7 +9216,7 @@
         <v>6.4397399999999994E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15">
       <c r="A7" s="32" t="s">
         <v>18</v>
       </c>
@@ -9064,7 +9224,7 @@
         <v>0.39335199999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="15">
       <c r="A8" s="32" t="s">
         <v>21</v>
       </c>
@@ -9080,6 +9240,213 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6537420D-1207-43EE-B3A1-8A7E1D1CB75B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="52"/>
+      <c r="B1" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="27.6">
+      <c r="A2" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="53">
+        <v>0.26347700000000002</v>
+      </c>
+      <c r="C2" s="54">
+        <v>0.32245000000000001</v>
+      </c>
+      <c r="D2" s="54">
+        <v>0.192131</v>
+      </c>
+      <c r="E2" s="54">
+        <v>0.33137299999999997</v>
+      </c>
+      <c r="F2" s="55">
+        <v>0.277673</v>
+      </c>
+      <c r="G2" s="55">
+        <v>0.23852499999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="53">
+        <v>3.5707200000000001E-2</v>
+      </c>
+      <c r="C3" s="54">
+        <v>0.15903400000000001</v>
+      </c>
+      <c r="D3" s="54">
+        <v>8.5563200000000006E-2</v>
+      </c>
+      <c r="E3" s="54">
+        <v>0.10716299999999999</v>
+      </c>
+      <c r="F3" s="55">
+        <v>0.16120699999999999</v>
+      </c>
+      <c r="G3" s="55">
+        <v>7.6639899999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="53">
+        <v>3.8541899999999997E-2</v>
+      </c>
+      <c r="C4" s="54">
+        <v>5.7736900000000001E-2</v>
+      </c>
+      <c r="D4" s="54">
+        <v>0.27891100000000002</v>
+      </c>
+      <c r="E4" s="54">
+        <v>5.8135300000000001E-2</v>
+      </c>
+      <c r="F4" s="55">
+        <v>3.1772800000000004E-2</v>
+      </c>
+      <c r="G4" s="55">
+        <v>3.0696599999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="53">
+        <v>0.45877299999999999</v>
+      </c>
+      <c r="C5" s="54">
+        <v>0.25053700000000001</v>
+      </c>
+      <c r="D5" s="54">
+        <v>0.34997200000000001</v>
+      </c>
+      <c r="E5" s="54">
+        <v>0.13347000000000001</v>
+      </c>
+      <c r="F5" s="55">
+        <v>0.134713</v>
+      </c>
+      <c r="G5" s="55">
+        <v>0.191916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="27.6">
+      <c r="A6" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="53">
+        <v>3.5458500000000004E-2</v>
+      </c>
+      <c r="C6" s="54">
+        <v>5.1121199999999999E-2</v>
+      </c>
+      <c r="D6" s="54">
+        <v>3.83608E-2</v>
+      </c>
+      <c r="E6" s="54">
+        <v>4.3516800000000001E-2</v>
+      </c>
+      <c r="F6" s="55">
+        <v>1.3107500000000001E-2</v>
+      </c>
+      <c r="G6" s="55">
+        <v>6.4397399999999994E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="53">
+        <v>0.15615699999999999</v>
+      </c>
+      <c r="C7" s="54">
+        <v>0.155168</v>
+      </c>
+      <c r="D7" s="54">
+        <v>2.7507500000000001E-2</v>
+      </c>
+      <c r="E7" s="54">
+        <v>0.323959</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.37993199999999999</v>
+      </c>
+      <c r="G7" s="55">
+        <v>0.39335199999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="53">
+        <v>1.18858E-2</v>
+      </c>
+      <c r="C8" s="54">
+        <v>3.9522300000000002E-3</v>
+      </c>
+      <c r="D8" s="54">
+        <v>2.75543E-2</v>
+      </c>
+      <c r="E8" s="54">
+        <v>2.3835800000000002E-3</v>
+      </c>
+      <c r="F8" s="55">
+        <v>1.59458E-3</v>
+      </c>
+      <c r="G8" s="55">
+        <v>4.4723499999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C8F5A9-FD81-4CD5-A93B-E2A92366F94E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -9087,15 +9454,15 @@
       <selection activeCell="D7" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="31.2">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -9109,7 +9476,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -9123,7 +9490,7 @@
         <v>91459</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -9137,7 +9504,7 @@
         <v>21376</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -9151,7 +9518,7 @@
         <v>11639</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.6">
       <c r="A5" s="9" t="s">
         <v>23</v>
       </c>
@@ -9165,7 +9532,7 @@
         <v>20108</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.6">
       <c r="A6" s="9" t="s">
         <v>50</v>
       </c>
@@ -9179,7 +9546,7 @@
         <v>193782</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.6">
       <c r="A7" s="9" t="s">
         <v>57</v>
       </c>
@@ -9199,7 +9566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5045AAAD-7A1A-42C3-8572-22A393E9AA9D}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -9207,16 +9574,16 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.36328125" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="18" t="s">
         <v>31</v>
       </c>
@@ -9239,7 +9606,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -9262,7 +9629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -9285,7 +9652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -9308,7 +9675,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -9331,7 +9698,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -9354,7 +9721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -9377,7 +9744,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -9405,26 +9772,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043F2D52-0DC5-49D1-854E-0E75D3795ABD}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.26953125" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" customWidth="1"/>
-    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="18.36328125" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" s="41" t="s">
         <v>31</v>
       </c>
@@ -9450,7 +9817,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="45" t="s">
         <v>16</v>
       </c>
@@ -9476,7 +9843,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="45" t="s">
         <v>20</v>
       </c>
@@ -9502,7 +9869,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="45" t="s">
         <v>18</v>
       </c>
@@ -9528,7 +9895,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="45" t="s">
         <v>17</v>
       </c>
@@ -9554,7 +9921,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="45" t="s">
         <v>15</v>
       </c>
@@ -9580,7 +9947,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="45" t="s">
         <v>19</v>
       </c>
@@ -9606,7 +9973,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="45" t="s">
         <v>21</v>
       </c>
@@ -9632,7 +9999,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="42"/>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -9644,7 +10011,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="43" t="s">
         <v>31</v>
       </c>
@@ -9670,7 +10037,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="44" t="s">
         <v>16</v>
       </c>
@@ -9696,7 +10063,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="44" t="s">
         <v>20</v>
       </c>
@@ -9722,7 +10089,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="44" t="s">
         <v>18</v>
       </c>
@@ -9748,7 +10115,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="44" t="s">
         <v>17</v>
       </c>
@@ -9774,7 +10141,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="44" t="s">
         <v>15</v>
       </c>
@@ -9800,7 +10167,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="44" t="s">
         <v>19</v>
       </c>
@@ -9826,7 +10193,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15" customHeight="1">
       <c r="A17" s="44" t="s">
         <v>21</v>
       </c>
@@ -9852,8 +10219,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15" customHeight="1"/>
+    <row r="20" spans="1:8">
       <c r="A20" s="18" t="s">
         <v>31</v>
       </c>
@@ -9876,7 +10243,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -9899,7 +10266,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -9922,7 +10289,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -9945,7 +10312,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -9968,7 +10335,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -9991,7 +10358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -10014,7 +10381,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -10037,7 +10404,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="18" t="s">
         <v>31</v>
       </c>
@@ -10060,7 +10427,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -10083,7 +10450,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -10106,7 +10473,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -10129,7 +10496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -10152,7 +10519,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -10175,7 +10542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -10198,7 +10565,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -10227,21 +10594,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D9752B-20C6-4797-82E8-FBA3F0E6167C}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="16"/>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
@@ -10249,7 +10616,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
@@ -10258,7 +10625,7 @@
       </c>
       <c r="C2" s="17"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
@@ -10267,7 +10634,7 @@
       </c>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
         <v>19</v>
       </c>
@@ -10276,7 +10643,7 @@
       </c>
       <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
         <v>16</v>
       </c>
@@ -10285,7 +10652,7 @@
       </c>
       <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3">
       <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
@@ -10294,7 +10661,7 @@
       </c>
       <c r="C6" s="17"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
@@ -10303,7 +10670,7 @@
       </c>
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3">
       <c r="A8" s="12" t="s">
         <v>21</v>
       </c>
@@ -10314,97 +10681,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{00D9752B-20C6-4797-82E8-FBA3F0E6167C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C8">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB718D3-C404-4D39-8DA3-A6344E204ED8}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.08984375" customWidth="1"/>
-    <col min="2" max="2" width="20.90625" customWidth="1"/>
-    <col min="5" max="5" width="17.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0.32245000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.15903400000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6">
-        <v>5.7736900000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.25053700000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="6">
-        <v>5.1121199999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.155168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6">
-        <v>3.9522300000000002E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{CBB718D3-C404-4D39-8DA3-A6344E204ED8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+    <sortState ref="A2:C8">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -10414,86 +10691,87 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7311EFB-2DE6-43C1-BB19-9086A9DDA371}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB718D3-C404-4D39-8DA3-A6344E204ED8}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="6">
-        <v>0.192131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.32245000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6">
-        <v>8.5563200000000006E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.15903400000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="6">
-        <v>0.27891100000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5.7736900000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6">
-        <v>0.34997200000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>0.25053700000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="6">
-        <v>3.83608E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>5.1121199999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="6">
-        <v>2.7507500000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>0.155168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6">
-        <v>2.75543E-2</v>
+        <v>3.9522300000000002E-3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{C7311EFB-2DE6-43C1-BB19-9086A9DDA371}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+  <autoFilter ref="A1:B1" xr:uid="{CBB718D3-C404-4D39-8DA3-A6344E204ED8}">
+    <sortState ref="A2:B8">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -10503,86 +10781,86 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AA5A83-BD6D-41DA-9982-1ACA03113A1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7311EFB-2DE6-43C1-BB19-9086A9DDA371}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="22.8">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="6">
-        <v>0.33137299999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.192131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6">
-        <v>0.10716299999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8.5563200000000006E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="6">
-        <v>5.8135300000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.27891100000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6">
-        <v>0.13347000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>0.34997200000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="22.8">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="6">
-        <v>4.3516800000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>3.83608E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="6">
-        <v>0.323959</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="23" x14ac:dyDescent="0.35">
+        <v>2.7507500000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6">
-        <v>2.3835800000000002E-3</v>
+        <v>2.75543E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{99AA5A83-BD6D-41DA-9982-1ACA03113A1A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
+  <autoFilter ref="A1:B1" xr:uid="{C7311EFB-2DE6-43C1-BB19-9086A9DDA371}">
+    <sortState ref="A2:B8">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -10592,95 +10870,86 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0970C1-54A1-466F-8B11-808A46DDE000}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AA5A83-BD6D-41DA-9982-1ACA03113A1A}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27" style="34" customWidth="1"/>
-    <col min="2" max="3" width="21.26953125" style="34" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="31"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="22.8">
+      <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33">
-        <v>0.277673</v>
-      </c>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
+      <c r="B2" s="6">
+        <v>0.33137299999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="33">
-        <v>0.16120699999999999</v>
-      </c>
-      <c r="C3" s="33"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="B3" s="6">
+        <v>0.10716299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="33">
-        <v>3.1772800000000004E-2</v>
-      </c>
-      <c r="C4" s="33"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="32" t="s">
+      <c r="B4" s="6">
+        <v>5.8135300000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="33">
-        <v>0.134713</v>
-      </c>
-      <c r="C5" s="33"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="B5" s="6">
+        <v>0.13347000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="22.8">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="33">
-        <v>1.3107500000000001E-2</v>
-      </c>
-      <c r="C6" s="33"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
+      <c r="B6" s="6">
+        <v>4.3516800000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="33">
-        <v>0.37993199999999999</v>
-      </c>
-      <c r="C7" s="33"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
+      <c r="B7" s="6">
+        <v>0.323959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="33">
-        <v>1.59458E-3</v>
-      </c>
-      <c r="C8" s="33"/>
+      <c r="B8" s="6">
+        <v>2.3835800000000002E-3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{FE0970C1-54A1-466F-8B11-808A46DDE000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
+  <autoFilter ref="A1:B1" xr:uid="{99AA5A83-BD6D-41DA-9982-1ACA03113A1A}">
+    <sortState ref="A2:B8">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>